<commit_message>
csv import + roles
</commit_message>
<xml_diff>
--- a/src/assets/šablona.xlsx
+++ b/src/assets/šablona.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ondra\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAA6BBDE-D0C7-4F15-9DA4-70BEF0A671DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98022C39-8A43-455B-9A1F-4734EB61BFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B70A2656-299F-4E93-BCC8-85FE9C4C13BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B70A2656-299F-4E93-BCC8-85FE9C4C13BD}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>type</t>
   </si>
@@ -52,12 +52,15 @@
   <si>
     <t>last_name</t>
   </si>
+  <si>
+    <t>role</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +77,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -83,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,17 +118,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,13 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC71092D-D460-431D-8390-A7295A2850A3}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,11 +497,20 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>